<commit_message>
Script SOLO y Manual
</commit_message>
<xml_diff>
--- a/dataframe pandas/Clasificación_y_métricas de soluciones.xlsx
+++ b/dataframe pandas/Clasificación_y_métricas de soluciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecnube1-my.sharepoint.com/personal/lsancho_itcr_ac_cr/Documents/INVESTIGACION/Poliglot/8 - Actividad intencionada/Análisis 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2d6bad750472d51/Documents/GitHub/poliglot/dataframe pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5562" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F9B8C75-E748-49AB-B123-68672D097F55}"/>
+  <xr:revisionPtr revIDLastSave="5566" documentId="11_7E4E55BF84DCCEE3ED7FF6F99031F45BFA722949" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88B92E9A-7EF0-4442-B8FA-24BF8A836A30}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoologico 1_vIAC" sheetId="6" r:id="rId1"/>
@@ -1469,7 +1469,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1511,11 +1511,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1769,7 +1764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1879,7 +1874,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1892,112 +1889,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="151">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -2235,6 +2131,54 @@
         <left/>
         <right/>
         <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -2557,6 +2501,54 @@
         <left/>
         <right/>
         <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom/>
       </border>
     </dxf>
@@ -3042,55 +3034,55 @@
   </sortState>
   <tableColumns count="28">
     <tableColumn id="1" xr3:uid="{56D3F157-C556-409A-81B8-8A57755A627D}" name="Carnet" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="28" xr3:uid="{1E997523-71CD-43E9-9116-C9A74FB868D5}" name="Nivel_Abstracción_MANUAL profes" totalsRowDxfId="3"/>
-    <tableColumn id="27" xr3:uid="{04D7FEEF-8BC1-4CB4-A902-B21E26B6B343}" name="Evaluación SOLO" totalsRowDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{D9CF57D0-036D-4FB8-A3BC-0A61EB0DD29C}" name="Nivel_Abstracción_ENCUESTA Inke" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{5AAF512F-6400-45ED-ACA0-7F4FEBC6E15E}" name="Clasificación" totalsRowDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{565BCD26-F575-4A88-942B-389A73A9982E}" name="Comentarios" totalsRowDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{C96BC0C6-9D9F-412D-BEA9-6FDD747E46B1}" name="LoCode" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{4CE3ADE3-AC86-4D70-9EC0-D3306CDD0397}" name="LoComments" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{7743901C-5A51-4952-B0B4-6BD99AA1A8A6}" name="NoFunctions" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{1E1D651B-4DBF-4627-B1A9-86D9F0812AD5}" name="ERL" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="8" xr3:uid="{0753FAAE-97F3-42EA-8D5C-7B11EEED0FC4}" name="IRL" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="9" xr3:uid="{EA71DD97-92F3-44FC-BF5F-FB2FBF0290D2}" name="IRC" dataDxfId="80" totalsRowDxfId="79">
+    <tableColumn id="28" xr3:uid="{1E997523-71CD-43E9-9116-C9A74FB868D5}" name="Nivel_Abstracción_MANUAL profes" totalsRowDxfId="92"/>
+    <tableColumn id="27" xr3:uid="{04D7FEEF-8BC1-4CB4-A902-B21E26B6B343}" name="Evaluación SOLO" totalsRowDxfId="91"/>
+    <tableColumn id="26" xr3:uid="{D9CF57D0-036D-4FB8-A3BC-0A61EB0DD29C}" name="Nivel_Abstracción_ENCUESTA Inke" totalsRowDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{5AAF512F-6400-45ED-ACA0-7F4FEBC6E15E}" name="Clasificación" totalsRowDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{565BCD26-F575-4A88-942B-389A73A9982E}" name="Comentarios" totalsRowDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{C96BC0C6-9D9F-412D-BEA9-6FDD747E46B1}" name="LoCode" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{4CE3ADE3-AC86-4D70-9EC0-D3306CDD0397}" name="LoComments" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{7743901C-5A51-4952-B0B4-6BD99AA1A8A6}" name="NoFunctions" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{1E1D651B-4DBF-4627-B1A9-86D9F0812AD5}" name="ERL" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{0753FAAE-97F3-42EA-8D5C-7B11EEED0FC4}" name="IRL" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{EA71DD97-92F3-44FC-BF5F-FB2FBF0290D2}" name="IRC" dataDxfId="77" totalsRowDxfId="76">
       <calculatedColumnFormula>Tabla1[[#This Row],[ERL]]+Tabla1[[#This Row],[IRL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C79AA6F0-BE2B-486B-8A60-DBE19A2F9033}" name="CC" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="11" xr3:uid="{CC90B57D-326C-4883-B48B-74D26B09BBFC}" name="TPFM" dataDxfId="76" totalsRowDxfId="75">
+    <tableColumn id="10" xr3:uid="{C79AA6F0-BE2B-486B-8A60-DBE19A2F9033}" name="CC" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="11" xr3:uid="{CC90B57D-326C-4883-B48B-74D26B09BBFC}" name="TPFM" dataDxfId="73" totalsRowDxfId="72">
       <calculatedColumnFormula>Tabla1[[#This Row],[LoCode]]/Tabla1[[#This Row],[NoFunctions]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{56413DEE-90FB-4281-9356-7E0C90A3C8E0}" name="IDC" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="13" xr3:uid="{9F6F9577-E33D-412F-A985-E50ACAD16969}" name="Valor general" dataDxfId="72" totalsRowDxfId="71">
+    <tableColumn id="12" xr3:uid="{56413DEE-90FB-4281-9356-7E0C90A3C8E0}" name="IDC" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="13" xr3:uid="{9F6F9577-E33D-412F-A985-E50ACAD16969}" name="Valor general" dataDxfId="69" totalsRowDxfId="68">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[CC]:[IDC]]) - Tabla1[[#This Row],[IRC]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6AA941FC-6B47-45AE-A4D3-929E2F837F2F}" name="Nivel de abstracción" dataDxfId="70" totalsRowDxfId="69">
+    <tableColumn id="14" xr3:uid="{6AA941FC-6B47-45AE-A4D3-929E2F837F2F}" name="Nivel de abstracción" dataDxfId="67" totalsRowDxfId="66">
       <calculatedColumnFormula>IF(P3 &lt; $G$49, "Alto", IF(P3 &lt; $G$51, "Medio", "Bajo"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{77EC9D60-6D43-4EBA-B953-C464380B8D38}" name="IPTFM" dataDxfId="68" totalsRowDxfId="67">
+    <tableColumn id="15" xr3:uid="{77EC9D60-6D43-4EBA-B953-C464380B8D38}" name="IPTFM" dataDxfId="65" totalsRowDxfId="64">
       <calculatedColumnFormula>1 - ((Tabla1[[#This Row],[TPFM]]- $N$50) / ($N$49 - $N$50))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{9EB55A6D-6E51-4B86-98B8-049321728E9B}" name="Coherencia en nomenclatura" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="17" xr3:uid="{143EA8DC-A538-49E9-B708-9AC256299540}" name="Comentarios2" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="18" xr3:uid="{517664B3-8BA8-457A-87ED-8C7820B35F26}" name="ICLC" dataDxfId="62" totalsRowDxfId="61">
+    <tableColumn id="16" xr3:uid="{9EB55A6D-6E51-4B86-98B8-049321728E9B}" name="Coherencia en nomenclatura" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="17" xr3:uid="{143EA8DC-A538-49E9-B708-9AC256299540}" name="Comentarios2" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="18" xr3:uid="{517664B3-8BA8-457A-87ED-8C7820B35F26}" name="ICLC" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>SUM(Tabla1[[#This Row],[IPTFM]:[Comentarios2]]) / 3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{4EF4417D-B595-476A-AA13-3923873EC1B6}" name="ICC" dataDxfId="60" totalsRowDxfId="59">
+    <tableColumn id="19" xr3:uid="{4EF4417D-B595-476A-AA13-3923873EC1B6}" name="ICC" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>Tabla1[[#This Row],[CC]]/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{38B1F1A2-67DE-402C-AF08-D329FB499366}" name="Valor general2" dataDxfId="58" totalsRowDxfId="57">
+    <tableColumn id="20" xr3:uid="{38B1F1A2-67DE-402C-AF08-D329FB499366}" name="Valor general2" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula xml:space="preserve"> (Tabla1[[#This Row],[ICLC]] + (1 - Tabla1[[#This Row],[ICC]])) / 2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{B85C086F-3B8F-4682-9B86-378AC6B64917}" name="Nivel de PA" dataDxfId="56" totalsRowDxfId="55">
+    <tableColumn id="21" xr3:uid="{B85C086F-3B8F-4682-9B86-378AC6B64917}" name="Nivel de PA" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula>IF(W3 &lt; $S$47, "Bajo", IF(W3 &lt; $S$49, "Medio", "Alto"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{F92B72AB-D162-404F-BBDE-D1E37D3FCD39}" name="INN" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="23" xr3:uid="{D897B942-4960-4BEC-A267-C1CA78DF927C}" name="Nivel de RD" dataDxfId="52" totalsRowDxfId="51">
+    <tableColumn id="22" xr3:uid="{F92B72AB-D162-404F-BBDE-D1E37D3FCD39}" name="INN" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="23" xr3:uid="{D897B942-4960-4BEC-A267-C1CA78DF927C}" name="Nivel de RD" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula>IF(Y3 &lt; $Y$47, "Bajo", IF(Y3 &gt;= $Y$49, "Alto", "Medio"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{6BB25B49-45FC-485B-8F42-2AD14F2000AF}" name="Valor general de PC" dataDxfId="50" totalsRowDxfId="49">
+    <tableColumn id="24" xr3:uid="{6BB25B49-45FC-485B-8F42-2AD14F2000AF}" name="Valor general de PC" dataDxfId="47" totalsRowDxfId="46">
       <calculatedColumnFormula>Tabla1[[#This Row],[Valor general]]-Tabla1[[#This Row],[Valor general2]]-Tabla1[[#This Row],[INN]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{352CEB45-F099-4B66-A28E-2229922A956D}" name="Nivel" dataDxfId="48" totalsRowDxfId="47">
+    <tableColumn id="25" xr3:uid="{352CEB45-F099-4B66-A28E-2229922A956D}" name="Nivel" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula>IF(Tabla1[[#This Row],[Valor general de PC]]&lt; $AA$49, "Alto", IF(Tabla1[[#This Row],[Valor general de PC]]&lt; $AA$51, "Medio", "Bajo"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3099,62 +3091,62 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C819D21-D9D5-4FCD-9299-F5178FA0FC7F}" name="Tabla14" displayName="Tabla14" ref="A2:AB48" totalsRowShown="0" headerRowDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7C819D21-D9D5-4FCD-9299-F5178FA0FC7F}" name="Tabla14" displayName="Tabla14" ref="A2:AB48" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A2:AB48" xr:uid="{88A4A5F1-8909-456D-BD8D-F726CDF06316}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F48">
     <sortCondition ref="A2:A48"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{D8D0A058-8862-42B8-8AFE-EB37200D5E0A}" name="Carnet" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="28" xr3:uid="{47BA99CB-A47D-424C-B895-92E0D11635C9}" name="Nivel_Abstracción_MANUAL profes" totalsRowDxfId="0"/>
-    <tableColumn id="27" xr3:uid="{B70CD460-FCF9-489A-9AB4-B0BD2C7227C9}" name="Evaluación SOLO" totalsRowDxfId="1"/>
-    <tableColumn id="26" xr3:uid="{000F2E4C-AA66-4628-BE00-F05B0E0D7FDF}" name="Nivel_Abstracción_ENCUESTA Inke" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B5226488-FF57-4A33-9E1C-9FD8AD66CCB2}" name="Clasificación" totalsRowDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{A3226F33-AD8D-4D4B-BA08-FFE777003AE3}" name="Comentarios" totalsRowDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{88B97310-9095-40C2-B2A7-48E9BBD1FAD3}" name="LoCode" totalsRowDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{ADA7AA67-925B-4E29-B5BA-C263CADA81BF}" name="LoComments" totalsRowDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{36024AD1-130B-4859-9A99-3E1B719FBB2A}" name="NoFunctions" totalsRowDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{373A420C-E52D-4781-A524-C1BB06CDBDBA}" name="ERL" totalsRowDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{77340BD5-3193-424C-89DC-ED2EE24A5153}" name="IRL" totalsRowDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{30BFF488-410C-4BB5-B33E-2DDFFF48968E}" name="IRC" dataDxfId="36" totalsRowDxfId="35">
+    <tableColumn id="1" xr3:uid="{D8D0A058-8862-42B8-8AFE-EB37200D5E0A}" name="Carnet" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="28" xr3:uid="{47BA99CB-A47D-424C-B895-92E0D11635C9}" name="Nivel_Abstracción_MANUAL profes" totalsRowDxfId="40"/>
+    <tableColumn id="27" xr3:uid="{B70CD460-FCF9-489A-9AB4-B0BD2C7227C9}" name="Evaluación SOLO" totalsRowDxfId="39"/>
+    <tableColumn id="26" xr3:uid="{000F2E4C-AA66-4628-BE00-F05B0E0D7FDF}" name="Nivel_Abstracción_ENCUESTA Inke" totalsRowDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{B5226488-FF57-4A33-9E1C-9FD8AD66CCB2}" name="Clasificación" totalsRowDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{A3226F33-AD8D-4D4B-BA08-FFE777003AE3}" name="Comentarios" totalsRowDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{88B97310-9095-40C2-B2A7-48E9BBD1FAD3}" name="LoCode" totalsRowDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{ADA7AA67-925B-4E29-B5BA-C263CADA81BF}" name="LoComments" totalsRowDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{36024AD1-130B-4859-9A99-3E1B719FBB2A}" name="NoFunctions" totalsRowDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{373A420C-E52D-4781-A524-C1BB06CDBDBA}" name="ERL" totalsRowDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{77340BD5-3193-424C-89DC-ED2EE24A5153}" name="IRL" totalsRowDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{30BFF488-410C-4BB5-B33E-2DDFFF48968E}" name="IRC" dataDxfId="30" totalsRowDxfId="29">
       <calculatedColumnFormula>Tabla14[[#This Row],[ERL]]+Tabla14[[#This Row],[IRL]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{FCB40734-2031-4642-B552-E5384E42A425}" name="CC" totalsRowDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{E901A4A4-463B-486D-8CB2-132A95F30209}" name="TPFM" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="10" xr3:uid="{FCB40734-2031-4642-B552-E5384E42A425}" name="CC" totalsRowDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{E901A4A4-463B-486D-8CB2-132A95F30209}" name="TPFM" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>Tabla14[[#This Row],[LoCode]]/Tabla14[[#This Row],[NoFunctions]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B52B1488-6E93-4B05-A14A-739BD9377439}" name="IDC" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{9B6D9185-7721-4F8F-828C-302747069C0E}" name="Valor general" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="12" xr3:uid="{B52B1488-6E93-4B05-A14A-739BD9377439}" name="IDC" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="13" xr3:uid="{9B6D9185-7721-4F8F-828C-302747069C0E}" name="Valor general" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>SUM(Tabla14[[#This Row],[CC]:[IDC]]) - Tabla14[[#This Row],[IRC]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C74CA72C-9850-433A-974B-A4E5ECD84450}" name="Nivel de abstracción" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="14" xr3:uid="{C74CA72C-9850-433A-974B-A4E5ECD84450}" name="Nivel de abstracción" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>IF(P3 &lt; $J$47, "Alto", IF(P3 &lt; $G$51, "Medio", "Bajo"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{5A96DE51-45ED-4AEB-B0F4-9612B4C449C9}" name="IPTFM" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="15" xr3:uid="{5A96DE51-45ED-4AEB-B0F4-9612B4C449C9}" name="IPTFM" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula>1 - ((Tabla14[[#This Row],[TPFM]]- $N$50) / ($N$47 - $N$50))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{3E735E8D-0C8E-4B37-98CB-504F08D23469}" name="Coherencia en nomenclatura" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{E5284601-0985-4223-ABEC-9F511EE4F411}" name="Comentarios2" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{B59AD9FE-DE4D-4CB6-9D06-034AB3D1CABD}" name="ICLC" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="16" xr3:uid="{3E735E8D-0C8E-4B37-98CB-504F08D23469}" name="Coherencia en nomenclatura" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{E5284601-0985-4223-ABEC-9F511EE4F411}" name="Comentarios2" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{B59AD9FE-DE4D-4CB6-9D06-034AB3D1CABD}" name="ICLC" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>SUM(Tabla14[[#This Row],[IPTFM]:[Comentarios2]]) / 3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{D63E74F4-107A-40E6-8D4E-642F7880039F}" name="ICC" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="19" xr3:uid="{D63E74F4-107A-40E6-8D4E-642F7880039F}" name="ICC" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>Tabla14[[#This Row],[CC]]/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{F7FC70D5-4F3E-42A8-84B8-8EADF5D1A1A1}" name="Valor general2" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="20" xr3:uid="{F7FC70D5-4F3E-42A8-84B8-8EADF5D1A1A1}" name="Valor general2" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula xml:space="preserve"> (Tabla14[[#This Row],[ICLC]] + (1 - Tabla14[[#This Row],[ICC]])) / 2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{552302A1-EC72-4EAE-9CDA-CA49E0A3186A}" name="Nivel de PA" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="21" xr3:uid="{552302A1-EC72-4EAE-9CDA-CA49E0A3186A}" name="Nivel de PA" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>IF(W3 &lt; $W$50, "Bajo", IF(W3 &lt; $W$52, "Medio", "Alto"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{7A31D3B6-21CE-470C-B9C1-E8BF15441CCE}" name="INN" totalsRowDxfId="11"/>
-    <tableColumn id="23" xr3:uid="{9DB5F818-2976-481A-AA73-0219EEFE9023}" name="Nivel de RD" dataDxfId="10">
+    <tableColumn id="22" xr3:uid="{7A31D3B6-21CE-470C-B9C1-E8BF15441CCE}" name="INN" totalsRowDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{9DB5F818-2976-481A-AA73-0219EEFE9023}" name="Nivel de RD" dataDxfId="4">
       <calculatedColumnFormula>IF(Y3 &lt; $Y$51, "Bajo", IF(Y3 &gt;= $Y$53, "Alto", "Medio"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{F97DFCC1-125C-4090-B058-CBE2C57E9CBD}" name="Valor general de PC" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="24" xr3:uid="{F97DFCC1-125C-4090-B058-CBE2C57E9CBD}" name="Valor general de PC" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>Tabla14[[#This Row],[Valor general]]-Tabla14[[#This Row],[Valor general2]]-Tabla14[[#This Row],[INN]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{DF435C8F-9408-46A4-B78D-448978D62B75}" name="Nivel" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="25" xr3:uid="{DF435C8F-9408-46A4-B78D-448978D62B75}" name="Nivel" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>IF(Tabla14[[#This Row],[Valor general de PC]]&lt; $AA$50, "Alto", IF(Tabla14[[#This Row],[Valor general de PC]]&lt; $AA$52, "Medio", "Bajo"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3930,7 +3922,7 @@
       <c r="AN1" s="93"/>
       <c r="AO1" s="93"/>
     </row>
-    <row r="2" spans="1:42" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -7370,9 +7362,9 @@
     </row>
     <row r="26" spans="1:42" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
@@ -16899,8 +16891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16955,7 +16947,7 @@
       <c r="AA1" s="93"/>
       <c r="AB1" s="93"/>
     </row>
-    <row r="2" spans="1:28" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -17045,9 +17037,9 @@
       <c r="A3" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
       <c r="E3" s="82"/>
       <c r="F3" s="82"/>
       <c r="G3" s="84">
@@ -18715,9 +18707,9 @@
     </row>
     <row r="26" spans="1:28" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="17"/>
@@ -20995,7 +20987,7 @@
       <c r="AA1" s="93"/>
       <c r="AB1" s="93"/>
     </row>
-    <row r="2" spans="1:28" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -23150,9 +23142,9 @@
     </row>
     <row r="26" spans="1:28" s="4" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
       <c r="L26" s="51"/>
       <c r="O26" s="51"/>
       <c r="P26" s="51"/>
@@ -26046,8 +26038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD16F839-500F-48D3-B26C-1D22F244C594}">
   <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26109,13 +26101,13 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="96" t="s">
+      <c r="D2" s="89" t="s">
         <v>138</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -29724,9 +29716,9 @@
       <c r="A48" s="44">
         <v>2024800990</v>
       </c>
-      <c r="B48" s="95"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="95"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="21" t="s">
         <v>42</v>
       </c>

</xml_diff>